<commit_message>
all plots fixed - hyptheses fixes - general fixes
</commit_message>
<xml_diff>
--- a/output/LUAD_statistics_acinar.xlsx
+++ b/output/LUAD_statistics_acinar.xlsx
@@ -54,18 +54,18 @@
     <t>capri_bic.SD.POSTERR</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -99,28 +99,28 @@
     <t>15</t>
   </si>
   <si>
+    <t>Mutation TP53</t>
+  </si>
+  <si>
     <t>Mutation KRAS</t>
   </si>
   <si>
-    <t>Mutation TP53</t>
-  </si>
-  <si>
     <t>Amplification TSC2</t>
   </si>
   <si>
     <t>NA</t>
   </si>
   <si>
+    <t>Deletion CDKN2A</t>
+  </si>
+  <si>
+    <t>Mutation STK11</t>
+  </si>
+  <si>
     <t>Amplification RIT1</t>
   </si>
   <si>
-    <t>Mutation STK11</t>
-  </si>
-  <si>
     <t>Mutation RB1</t>
-  </si>
-  <si>
-    <t>Deletion CDKN2A</t>
   </si>
   <si>
     <t>Deletion MET</t>
@@ -287,37 +287,37 @@
         <v>32</v>
       </c>
       <c r="D2" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="E2" t="n">
         <v>2.0</v>
       </c>
       <c r="F2" t="n">
-        <v>1.80728584332411E-10</v>
+        <v>4.38795826699421E-12</v>
       </c>
       <c r="G2" t="n">
-        <v>1.40060582134077E-12</v>
+        <v>1.74974974000228E-14</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0833333333333333</v>
+        <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>60.0</v>
+        <v>50.0</v>
       </c>
       <c r="J2" t="n">
         <v>100.0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.15</v>
+        <v>0.125</v>
       </c>
       <c r="L2" t="n">
-        <v>0.04370036867375631</v>
+        <v>0.0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1625</v>
+        <v>0.125</v>
       </c>
       <c r="N2" t="n">
-        <v>0.052704627669473</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -325,7 +325,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
@@ -346,22 +346,22 @@
         <v>0.0178571428571429</v>
       </c>
       <c r="I3" t="n">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
       <c r="J3" t="n">
         <v>100.0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4</v>
+        <v>0.425</v>
       </c>
       <c r="L3" t="n">
-        <v>0.06718548123582124</v>
+        <v>0.026352313834736494</v>
       </c>
       <c r="M3" t="n">
-        <v>0.4</v>
+        <v>0.41875</v>
       </c>
       <c r="N3" t="n">
-        <v>0.052704627669473</v>
+        <v>0.0421842848569096</v>
       </c>
     </row>
     <row r="4">
@@ -375,37 +375,37 @@
         <v>34</v>
       </c>
       <c r="D4" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="E4" t="n">
         <v>2.0</v>
       </c>
       <c r="F4" t="n">
-        <v>1.08720193504961E-11</v>
+        <v>1.80728584332411E-10</v>
       </c>
       <c r="G4" t="n">
-        <v>1.39570418788465E-12</v>
+        <v>1.40060582134077E-12</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="I4" t="n">
-        <v>50.0</v>
+        <v>30.0</v>
       </c>
       <c r="J4" t="n">
         <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.125</v>
+        <v>0.1625</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0</v>
+        <v>0.05270462766947299</v>
       </c>
       <c r="M4" t="n">
-        <v>0.125</v>
+        <v>0.15625</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0</v>
+        <v>0.0441941738241592</v>
       </c>
     </row>
     <row r="5">
@@ -413,7 +413,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -425,16 +425,16 @@
         <v>2.0</v>
       </c>
       <c r="F5" t="n">
-        <v>4.38795826699421E-12</v>
+        <v>1.08720193504961E-11</v>
       </c>
       <c r="G5" t="n">
-        <v>1.74974974000228E-14</v>
+        <v>1.39570418788465E-12</v>
       </c>
       <c r="H5" t="n">
         <v>0.0</v>
       </c>
       <c r="I5" t="n">
-        <v>40.0</v>
+        <v>30.0</v>
       </c>
       <c r="J5" t="n">
         <v>100.0</v>
@@ -490,10 +490,10 @@
         <v>0.0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.125</v>
+        <v>0.1125</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0</v>
+        <v>0.0395284707521047</v>
       </c>
     </row>
     <row r="7">
@@ -636,7 +636,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" t="e">
         <v>#NUM!</v>
@@ -768,7 +768,7 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" t="e">
         <v>#NUM!</v>
@@ -792,10 +792,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K13" t="n">
-        <v>0.53125</v>
+        <v>0.5875</v>
       </c>
       <c r="L13" t="n">
-        <v>0.06750771560841522</v>
+        <v>0.10290907529357057</v>
       </c>
       <c r="M13" t="e">
         <v>#NUM!</v>
@@ -880,10 +880,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K15" t="n">
-        <v>0.81875</v>
+        <v>0.83125</v>
       </c>
       <c r="L15" t="n">
-        <v>0.09969571761671166</v>
+        <v>0.12517349071499834</v>
       </c>
       <c r="M15" t="e">
         <v>#NUM!</v>
@@ -1002,37 +1002,37 @@
         <v>32</v>
       </c>
       <c r="D2" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="E2" t="n">
         <v>2.0</v>
       </c>
       <c r="F2" t="n">
-        <v>1.80728584332411E-10</v>
+        <v>4.38795826699421E-12</v>
       </c>
       <c r="G2" t="n">
-        <v>1.40060582134077E-12</v>
+        <v>1.74974974000228E-14</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0833333333333333</v>
+        <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>60.0</v>
+        <v>50.0</v>
       </c>
       <c r="J2" t="n">
         <v>100.0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.15</v>
+        <v>0.125</v>
       </c>
       <c r="L2" t="n">
-        <v>0.04370036867375631</v>
+        <v>0.0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1375</v>
+        <v>0.125</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0263523138347365</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -1040,7 +1040,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>33</v>
@@ -1061,22 +1061,22 @@
         <v>0.0178571428571429</v>
       </c>
       <c r="I3" t="n">
-        <v>60.0</v>
+        <v>40.0</v>
       </c>
       <c r="J3" t="n">
         <v>100.0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4</v>
+        <v>0.425</v>
       </c>
       <c r="L3" t="n">
-        <v>0.06718548123582124</v>
+        <v>0.026352313834736494</v>
       </c>
       <c r="M3" t="n">
-        <v>0.425</v>
+        <v>0.4125</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0395284707521047</v>
+        <v>0.0437003686737563</v>
       </c>
     </row>
     <row r="4">
@@ -1090,31 +1090,31 @@
         <v>34</v>
       </c>
       <c r="D4" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="E4" t="n">
         <v>2.0</v>
       </c>
       <c r="F4" t="n">
-        <v>1.08720193504961E-11</v>
+        <v>1.80728584332411E-10</v>
       </c>
       <c r="G4" t="n">
-        <v>1.39570418788465E-12</v>
+        <v>1.40060582134077E-12</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="I4" t="n">
-        <v>50.0</v>
+        <v>30.0</v>
       </c>
       <c r="J4" t="n">
         <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.125</v>
+        <v>0.1625</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0</v>
+        <v>0.05270462766947299</v>
       </c>
       <c r="M4" t="n">
         <v>0.125</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -1140,16 +1140,16 @@
         <v>2.0</v>
       </c>
       <c r="F5" t="n">
-        <v>4.38795826699421E-12</v>
+        <v>1.08720193504961E-11</v>
       </c>
       <c r="G5" t="n">
-        <v>1.74974974000228E-14</v>
+        <v>1.39570418788465E-12</v>
       </c>
       <c r="H5" t="n">
         <v>0.0</v>
       </c>
       <c r="I5" t="n">
-        <v>40.0</v>
+        <v>30.0</v>
       </c>
       <c r="J5" t="n">
         <v>100.0</v>
@@ -1172,7 +1172,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
@@ -1216,7 +1216,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>36</v>
@@ -1351,7 +1351,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" t="e">
         <v>#NUM!</v>
@@ -1483,7 +1483,7 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" t="e">
         <v>#NUM!</v>
@@ -1507,10 +1507,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K13" t="n">
-        <v>0.53125</v>
+        <v>0.5875</v>
       </c>
       <c r="L13" t="n">
-        <v>0.06750771560841522</v>
+        <v>0.10290907529357057</v>
       </c>
       <c r="M13" t="e">
         <v>#NUM!</v>
@@ -1595,10 +1595,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K15" t="n">
-        <v>0.81875</v>
+        <v>0.83125</v>
       </c>
       <c r="L15" t="n">
-        <v>0.09969571761671166</v>
+        <v>0.12517349071499834</v>
       </c>
       <c r="M15" t="e">
         <v>#NUM!</v>

</xml_diff>